<commit_message>
clase 6 10 09 24 completada con codigos comentados
</commit_message>
<xml_diff>
--- a/Ejercicios en clase/Clase 6 10 09 24/formulas 10 09 24.xlsx
+++ b/Ejercicios en clase/Clase 6 10 09 24/formulas 10 09 24.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/931d574390e6cf0b/Documentos/ITS Semestre 11/VISION COMPUTACIONAL/Ejercicios en clase/Clase 6 10 9 24/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/931d574390e6cf0b/Documentos/ITS Semestre 11/VISION COMPUTACIONAL/Ejercicios en clase/Clase 6 10 09 24/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="221" documentId="8_{06E41512-9289-4F77-8C09-E7592327420D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C31EE24D-3B20-42CA-9B1F-625F072C910F}"/>
+  <xr:revisionPtr revIDLastSave="228" documentId="8_{06E41512-9289-4F77-8C09-E7592327420D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92088E45-897B-48F8-92B2-FB7BE0CE469F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6D742EB4-82D1-4DCD-83C8-4CCD18FAFC90}"/>
   </bookViews>
@@ -1016,7 +1016,7 @@
   <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="121" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1805,7 +1805,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2331,7 +2331,7 @@
         <v>1</v>
       </c>
       <c r="H29" s="8">
-        <f t="shared" si="1"/>
+        <f>G29/14</f>
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="I29" s="1">
@@ -2398,7 +2398,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>